<commit_message>
adatp the design matrix and tables for the nf-pipeline
</commit_message>
<xml_diff>
--- a/exp_design/sampleInfo_R7708.xlsx
+++ b/exp_design/sampleInfo_R7708.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philipp.dexheimer/Desktop/RNAseq RNAiD experiment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/groups/cochella/jiwang/Projects/Philipp/smallRNA_analysis_philipp/exp_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F76635F4-F6E2-EC42-B5BF-785ED5B26556}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E163E2-B569-DD46-8830-BE1C7B6F18E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1D4C5632-9F48-134E-BE42-B2A0D81629DE}"/>
+    <workbookView xWindow="36760" yWindow="-4020" windowWidth="28800" windowHeight="17540" xr2:uid="{1D4C5632-9F48-134E-BE42-B2A0D81629DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
   <si>
     <t>Strain</t>
   </si>
@@ -199,61 +193,13 @@
   </si>
   <si>
     <t>Standard</t>
-  </si>
-  <si>
-    <t>2-cell</t>
-  </si>
-  <si>
-    <t>control</t>
-  </si>
-  <si>
-    <t>A1.1</t>
-  </si>
-  <si>
-    <t>M7870</t>
-  </si>
-  <si>
-    <t>IDX1</t>
-  </si>
-  <si>
-    <t>A1.2</t>
-  </si>
-  <si>
-    <t>IDX2</t>
-  </si>
-  <si>
-    <t>A2.1</t>
-  </si>
-  <si>
-    <t>IDX3</t>
-  </si>
-  <si>
-    <t>A2.2</t>
-  </si>
-  <si>
-    <t>A3.1</t>
-  </si>
-  <si>
-    <t>7hps</t>
-  </si>
-  <si>
-    <t>A4.1</t>
-  </si>
-  <si>
-    <t>A8.1</t>
-  </si>
-  <si>
-    <t>A9.1</t>
-  </si>
-  <si>
-    <t>A9.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -265,12 +211,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -388,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,9 +361,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -740,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B80B28D-CFEC-184E-A081-A8ABFF29CB2C}">
-  <dimension ref="B1:I28"/>
+  <dimension ref="B1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J29"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1165,267 +1102,6 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="5">
-        <v>84788</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="5">
-        <v>84789</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="5">
-        <v>84790</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="5">
-        <v>84791</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="5">
-        <v>84792</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="5">
-        <v>84793</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="5">
-        <v>84794</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="5">
-        <v>84795</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="9">
-        <v>84796</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>